<commit_message>
Add entry about network port internal and global listening, Nginx entry on how to listen to 2 host name on the same port 80
</commit_message>
<xml_diff>
--- a/nginx.xlsx
+++ b/nginx.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>Language</t>
   </si>
@@ -63,6 +63,64 @@
   </si>
   <si>
     <t>Proxy x directives</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t># NGINX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>## Check version</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>`whereis nginx`  // get the bin folder
+`/usr/sbin/nginx -v`  // say the bin is at /usr/sbin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>## Config Related File</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>## Multi Server Block Listening Same Port</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">There are 3 file/ folder related by default:
+1. /etc/nginx/nginx.conf
+    - The general conf, states properties like log, the sub-config files and etc.
+    - Usually sub-config files are  _/etc/nginx/conf.d/*.conf_ and _/etc/sites-enabled/*_
+1. /etc/nginx/sites-enabled/*
+    - In this folder, we should place soft link that point to ../sites-avalible (represent the activation)
+    - `sudo ln -s ./sites-available/myles.mobi ./sites-enabled/myles.mobi`
+1. /etc/nginx/sites-available/*
+    - Place all config that is available
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_ref: http://stackoverflow.com/questions/33055212/nginx-multiple-server-blocks-listening-to-same-port_
+This situation can be happened when we want to distribute request for different host(www or ftp or api…) from 80 to diff port.
+1. First we need to accept the new host on DNS (set A record with new host like api) to the same IP address
+1. In sites-available folder create **2** different config file say comments.myles.mobi and myles.mobi
+1. `cat myles.mobi`
+server {
+    listen 80;
+    server_name comments.myles.mobi
+    location / {
+        proxy_pass http://lcoalhost:8080;
+        proxy... (other setting)
+    }
+}
+1. `cat comments.myles.mobi`
+server {
+    listen 80;
+    server_name myles.mobi;
+    ....
+}
+1. Activate this 2 config in sites-enable folder 
+* Note: dont put in one config file, nginx will not be able to boot and return say 80 Address is already in use error mesage.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -439,17 +497,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="70.77734375" style="1" customWidth="1"/>
     <col min="4" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -464,7 +522,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="57" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -475,7 +533,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="69" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -486,7 +544,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="69" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -495,6 +553,39 @@
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="138" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="358.8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -510,7 +601,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -523,7 +614,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>